<commit_message>
Adiciona coluna de status de validação e remove arquivo de relatório desnecessário.
</commit_message>
<xml_diff>
--- a/validacao_mtm_final.xlsx
+++ b/validacao_mtm_final.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,11 @@
           <t>validacao_b3</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>status_validacao</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,6 +537,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -571,6 +581,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -610,6 +625,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -649,6 +669,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -688,6 +713,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -727,6 +757,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -766,6 +801,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -805,6 +845,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -844,6 +889,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -883,6 +933,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -922,6 +977,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -961,6 +1021,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1000,6 +1065,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1039,6 +1109,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1078,6 +1153,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1117,6 +1197,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1156,6 +1241,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1195,6 +1285,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1234,6 +1329,11 @@
           <t>Sucesso</t>
         </is>
       </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1271,6 +1371,11 @@
       <c r="K21" t="inlineStr">
         <is>
           <t>Sucesso</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>ERRO</t>
         </is>
       </c>
     </row>

</xml_diff>